<commit_message>
Fix component identifiers for JLCPCB
</commit_message>
<xml_diff>
--- a/Project Outputs for MICA-Glove-Carpus/BOM/Bill of Materials-MICA-Glove-Carpus.xlsx
+++ b/Project Outputs for MICA-Glove-Carpus/BOM/Bill of Materials-MICA-Glove-Carpus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\x-io\Services\MICA Lab\MICA-Glove-Carpus\Project Outputs for MICA-Glove-Carpus\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{485A8B26-D15B-4CFE-9B25-078EF26269FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BFAC037-FA45-4E5D-BCFD-ABA7F9B6CA87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5670" yWindow="1810" windowWidth="20850" windowHeight="18990" xr2:uid="{E6E690D2-158F-493D-9569-8823097D0084}"/>
+    <workbookView xWindow="5670" yWindow="1810" windowWidth="20850" windowHeight="18990" xr2:uid="{2FF05930-B5F1-4EF6-9091-605997479037}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-MICA-Glove-Ca" sheetId="1" r:id="rId1"/>
@@ -66,19 +66,19 @@
     <t>100nF</t>
   </si>
   <si>
-    <t>C21, C22, CH1 C23, CH1 C24, CH2 C23, CH2 C24, CH3 C23, CH3 C24, CH4 C23, CH4 C24, CH5 C23, CH5 C24</t>
+    <t>C21, C22, CH1_C23, CH1_C24, CH2_C23, CH2_C24, CH3_C23, CH3_C24, CH4_C23, CH4_C24, CH5_C23, CH5_C24</t>
   </si>
   <si>
     <t>1uF</t>
   </si>
   <si>
-    <t>CH1 J2, CH2 J2, CH3 J2, CH4 J2, CH5 J2</t>
+    <t>CH1_J2, CH2_J2, CH3_J2, CH4_J2, CH5_J2</t>
   </si>
   <si>
     <t>Molex 502426-2030</t>
   </si>
   <si>
-    <t>CH1 R7, CH1 R8, CH2 R7, CH2 R8, CH3 R7, CH3 R8, CH4 R7, CH4 R8, CH5 R7, CH5 R8, R3, R4, R5, R6</t>
+    <t>CH1_R7, CH1_R8, CH2_R7, CH2_R8, CH3_R7, CH3_R8, CH4_R7, CH4_R8, CH5_R7, CH5_R8, R3, R4, R5, R6</t>
   </si>
   <si>
     <t>4.7kR</t>
@@ -87,7 +87,7 @@
     <t>Resistor 0402</t>
   </si>
   <si>
-    <t>CH1 U9, CH2 U9, CH3 U9, CH4 U9, CH5 U9, U7</t>
+    <t>CH1_U9, CH2_U9, CH3_U9, CH4_U9, CH5_U9, U7</t>
   </si>
   <si>
     <t>SN74LVC1G97DRL</t>
@@ -550,7 +550,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2CF9CFF-7479-43D4-8C7A-698A313933A2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6FEF13E-3224-4BA4-AE36-3D3FF858D3DD}">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>